<commit_message>
Results for 10, 30 and 50 dimensions
</commit_message>
<xml_diff>
--- a/cec2017real-master/code/results_memeticARO/results_cec2017_10.xlsx
+++ b/cec2017real-master/code/results_memeticARO/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>593446200</v>
+        <v>4262026000</v>
       </c>
       <c r="D2" t="n">
-        <v>38033540</v>
+        <v>32016800000</v>
       </c>
       <c r="E2" t="n">
-        <v>41136.91</v>
+        <v>23912.55</v>
       </c>
       <c r="F2" t="n">
-        <v>412.7016</v>
+        <v>3061.992</v>
       </c>
       <c r="G2" t="n">
-        <v>139.1789</v>
+        <v>97.70949</v>
       </c>
       <c r="H2" t="n">
-        <v>97.13906</v>
+        <v>72.41793</v>
       </c>
       <c r="I2" t="n">
-        <v>114.4133</v>
+        <v>165.1325</v>
       </c>
       <c r="J2" t="n">
-        <v>79.70996</v>
+        <v>110.9142</v>
       </c>
       <c r="K2" t="n">
-        <v>2561.524</v>
+        <v>5690.49</v>
       </c>
       <c r="L2" t="n">
-        <v>1899.686</v>
+        <v>1835.97</v>
       </c>
       <c r="M2" t="n">
-        <v>91.76352</v>
+        <v>2040.547</v>
       </c>
       <c r="N2" t="n">
-        <v>12987360</v>
+        <v>17979150</v>
       </c>
       <c r="O2" t="n">
-        <v>15818.59</v>
+        <v>190336.5</v>
       </c>
       <c r="P2" t="n">
-        <v>1229.713</v>
+        <v>1802.758</v>
       </c>
       <c r="Q2" t="n">
-        <v>7705.381</v>
+        <v>53228.6</v>
       </c>
       <c r="R2" t="n">
-        <v>1119.639</v>
+        <v>440.3155</v>
       </c>
       <c r="S2" t="n">
-        <v>134.0211</v>
+        <v>108.603</v>
       </c>
       <c r="T2" t="n">
-        <v>1726570</v>
+        <v>219283.2</v>
       </c>
       <c r="U2" t="n">
-        <v>22406.91</v>
+        <v>125998</v>
       </c>
       <c r="V2" t="n">
-        <v>327.3973</v>
+        <v>360.7582</v>
       </c>
       <c r="W2" t="n">
-        <v>335.7215</v>
+        <v>111.0752</v>
       </c>
       <c r="X2" t="n">
         <v>1438.781</v>
       </c>
       <c r="Y2" t="n">
-        <v>363.6429</v>
+        <v>378.2358</v>
       </c>
       <c r="Z2" t="n">
-        <v>394.0597</v>
+        <v>404.6457</v>
       </c>
       <c r="AA2" t="n">
-        <v>554.3973</v>
+        <v>462.8941</v>
       </c>
       <c r="AB2" t="n">
-        <v>2118.738</v>
+        <v>2096.945</v>
       </c>
       <c r="AC2" t="n">
-        <v>448.1447</v>
+        <v>417.976</v>
       </c>
       <c r="AD2" t="n">
-        <v>780.7963999999999</v>
+        <v>699.5477</v>
       </c>
       <c r="AE2" t="n">
-        <v>448.5666</v>
+        <v>654.6838</v>
       </c>
       <c r="AF2" t="n">
-        <v>882863.3</v>
+        <v>881076.3</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>322402700</v>
+        <v>363219400</v>
       </c>
       <c r="D3" t="n">
-        <v>15458950</v>
+        <v>1474873000</v>
       </c>
       <c r="E3" t="n">
-        <v>36147.83</v>
+        <v>23877.51</v>
       </c>
       <c r="F3" t="n">
-        <v>165.7005</v>
+        <v>64.27508</v>
       </c>
       <c r="G3" t="n">
-        <v>79.81795</v>
+        <v>66.64358</v>
       </c>
       <c r="H3" t="n">
-        <v>53.48201</v>
+        <v>24.8669</v>
       </c>
       <c r="I3" t="n">
-        <v>104.0044</v>
+        <v>148.5461</v>
       </c>
       <c r="J3" t="n">
-        <v>65.90928</v>
+        <v>41.79208</v>
       </c>
       <c r="K3" t="n">
-        <v>2226.712</v>
+        <v>5690.49</v>
       </c>
       <c r="L3" t="n">
-        <v>1802.514</v>
+        <v>1354.686</v>
       </c>
       <c r="M3" t="n">
-        <v>91.76352</v>
+        <v>456.7292</v>
       </c>
       <c r="N3" t="n">
-        <v>5726372</v>
+        <v>14436320</v>
       </c>
       <c r="O3" t="n">
-        <v>15818.59</v>
+        <v>61002.24</v>
       </c>
       <c r="P3" t="n">
-        <v>1140.173</v>
+        <v>1153.221</v>
       </c>
       <c r="Q3" t="n">
-        <v>2598.249</v>
+        <v>9346.781999999999</v>
       </c>
       <c r="R3" t="n">
-        <v>216.8931</v>
+        <v>242.0612</v>
       </c>
       <c r="S3" t="n">
-        <v>127.8872</v>
+        <v>86.64427000000001</v>
       </c>
       <c r="T3" t="n">
-        <v>403184.5</v>
+        <v>173671.6</v>
       </c>
       <c r="U3" t="n">
-        <v>22406.91</v>
+        <v>37217.65</v>
       </c>
       <c r="V3" t="n">
-        <v>203.8021</v>
+        <v>124.0627</v>
       </c>
       <c r="W3" t="n">
-        <v>288.0186</v>
+        <v>109.833</v>
       </c>
       <c r="X3" t="n">
         <v>1438.781</v>
       </c>
       <c r="Y3" t="n">
-        <v>337.2127</v>
+        <v>340.8733</v>
       </c>
       <c r="Z3" t="n">
-        <v>386.9504</v>
+        <v>404.6457</v>
       </c>
       <c r="AA3" t="n">
-        <v>485.8191</v>
+        <v>458.6408</v>
       </c>
       <c r="AB3" t="n">
-        <v>2118.738</v>
+        <v>1497.518</v>
       </c>
       <c r="AC3" t="n">
-        <v>412.2065</v>
+        <v>411.14</v>
       </c>
       <c r="AD3" t="n">
-        <v>675.157</v>
+        <v>666.5614</v>
       </c>
       <c r="AE3" t="n">
-        <v>448.5666</v>
+        <v>458.7278</v>
       </c>
       <c r="AF3" t="n">
-        <v>882543.6</v>
+        <v>881076.3</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>322402700</v>
+        <v>256235500</v>
       </c>
       <c r="D4" t="n">
-        <v>15458950</v>
+        <v>392846400</v>
       </c>
       <c r="E4" t="n">
-        <v>26983.05</v>
+        <v>23877.51</v>
       </c>
       <c r="F4" t="n">
-        <v>80.96892</v>
+        <v>64.27508</v>
       </c>
       <c r="G4" t="n">
-        <v>67.73058</v>
+        <v>66.64358</v>
       </c>
       <c r="H4" t="n">
-        <v>39.94558</v>
+        <v>24.8669</v>
       </c>
       <c r="I4" t="n">
-        <v>104.0044</v>
+        <v>115.2115</v>
       </c>
       <c r="J4" t="n">
-        <v>65.90928</v>
+        <v>41.79208</v>
       </c>
       <c r="K4" t="n">
-        <v>1550.045</v>
+        <v>3259.06</v>
       </c>
       <c r="L4" t="n">
-        <v>1802.514</v>
+        <v>1354.686</v>
       </c>
       <c r="M4" t="n">
-        <v>91.76352</v>
+        <v>456.7292</v>
       </c>
       <c r="N4" t="n">
-        <v>5726372</v>
+        <v>14436320</v>
       </c>
       <c r="O4" t="n">
-        <v>15818.59</v>
+        <v>8566.797</v>
       </c>
       <c r="P4" t="n">
-        <v>1140.173</v>
+        <v>274.5239</v>
       </c>
       <c r="Q4" t="n">
-        <v>2598.249</v>
+        <v>2923.442</v>
       </c>
       <c r="R4" t="n">
-        <v>216.8931</v>
+        <v>242.0612</v>
       </c>
       <c r="S4" t="n">
-        <v>127.8872</v>
+        <v>86.64427000000001</v>
       </c>
       <c r="T4" t="n">
-        <v>276957.4</v>
+        <v>57188.54</v>
       </c>
       <c r="U4" t="n">
-        <v>22406.91</v>
+        <v>30219.88</v>
       </c>
       <c r="V4" t="n">
-        <v>176.3947</v>
+        <v>124.0627</v>
       </c>
       <c r="W4" t="n">
-        <v>266.1632</v>
+        <v>109.833</v>
       </c>
       <c r="X4" t="n">
         <v>1438.781</v>
       </c>
       <c r="Y4" t="n">
-        <v>334.5619</v>
+        <v>339.819</v>
       </c>
       <c r="Z4" t="n">
-        <v>386.626</v>
+        <v>402.4946</v>
       </c>
       <c r="AA4" t="n">
-        <v>481.4713</v>
+        <v>437.8539</v>
       </c>
       <c r="AB4" t="n">
-        <v>1989.798</v>
+        <v>1497.518</v>
       </c>
       <c r="AC4" t="n">
-        <v>399.1537</v>
+        <v>405.2154</v>
       </c>
       <c r="AD4" t="n">
-        <v>564.0166</v>
+        <v>666.5614</v>
       </c>
       <c r="AE4" t="n">
-        <v>399.7381</v>
+        <v>437.9849</v>
       </c>
       <c r="AF4" t="n">
-        <v>882543.6</v>
+        <v>881076.3</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>123373500</v>
+        <v>85805270</v>
       </c>
       <c r="D5" t="n">
-        <v>15458950</v>
+        <v>221955800</v>
       </c>
       <c r="E5" t="n">
-        <v>26983.05</v>
+        <v>18559.01</v>
       </c>
       <c r="F5" t="n">
-        <v>80.96892</v>
+        <v>55.24582</v>
       </c>
       <c r="G5" t="n">
-        <v>56.71194</v>
+        <v>48.46137</v>
       </c>
       <c r="H5" t="n">
-        <v>36.90042</v>
+        <v>24.8669</v>
       </c>
       <c r="I5" t="n">
-        <v>104.0044</v>
+        <v>115.2115</v>
       </c>
       <c r="J5" t="n">
-        <v>63.67987</v>
+        <v>41.79208</v>
       </c>
       <c r="K5" t="n">
-        <v>1550.045</v>
+        <v>157.3232</v>
       </c>
       <c r="L5" t="n">
-        <v>997.6338</v>
+        <v>1354.686</v>
       </c>
       <c r="M5" t="n">
-        <v>91.76352</v>
+        <v>160.5773</v>
       </c>
       <c r="N5" t="n">
-        <v>5726372</v>
+        <v>9728719</v>
       </c>
       <c r="O5" t="n">
-        <v>10588.75</v>
+        <v>8566.797</v>
       </c>
       <c r="P5" t="n">
-        <v>1140.173</v>
+        <v>274.5239</v>
       </c>
       <c r="Q5" t="n">
-        <v>2598.249</v>
+        <v>2170.566</v>
       </c>
       <c r="R5" t="n">
-        <v>216.8931</v>
+        <v>137.1645</v>
       </c>
       <c r="S5" t="n">
-        <v>95.34456</v>
+        <v>86.64427000000001</v>
       </c>
       <c r="T5" t="n">
-        <v>110059.1</v>
+        <v>57188.54</v>
       </c>
       <c r="U5" t="n">
-        <v>541.2913</v>
+        <v>30219.88</v>
       </c>
       <c r="V5" t="n">
-        <v>133.3401</v>
+        <v>124.0627</v>
       </c>
       <c r="W5" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X5" t="n">
-        <v>1438.781</v>
+        <v>180.3007</v>
       </c>
       <c r="Y5" t="n">
-        <v>334.5619</v>
+        <v>339.819</v>
       </c>
       <c r="Z5" t="n">
-        <v>370.5425</v>
+        <v>395.3369</v>
       </c>
       <c r="AA5" t="n">
-        <v>457.2187</v>
+        <v>437.8539</v>
       </c>
       <c r="AB5" t="n">
-        <v>949.353</v>
+        <v>920.4052</v>
       </c>
       <c r="AC5" t="n">
-        <v>399.1537</v>
+        <v>402.3601</v>
       </c>
       <c r="AD5" t="n">
-        <v>451.3176</v>
+        <v>666.5614</v>
       </c>
       <c r="AE5" t="n">
-        <v>355.9814</v>
+        <v>420.872</v>
       </c>
       <c r="AF5" t="n">
-        <v>882543.6</v>
+        <v>881076.3</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>91387400</v>
+        <v>27668500</v>
       </c>
       <c r="D6" t="n">
-        <v>15458950</v>
+        <v>89439790</v>
       </c>
       <c r="E6" t="n">
-        <v>22118.34</v>
+        <v>18559.01</v>
       </c>
       <c r="F6" t="n">
-        <v>28.42854</v>
+        <v>42.99143</v>
       </c>
       <c r="G6" t="n">
-        <v>56.71194</v>
+        <v>48.46137</v>
       </c>
       <c r="H6" t="n">
-        <v>27.31665</v>
+        <v>21.9057</v>
       </c>
       <c r="I6" t="n">
-        <v>74.63590000000001</v>
+        <v>115.2115</v>
       </c>
       <c r="J6" t="n">
-        <v>51.4392</v>
+        <v>41.79208</v>
       </c>
       <c r="K6" t="n">
-        <v>405.2997</v>
+        <v>157.3232</v>
       </c>
       <c r="L6" t="n">
-        <v>997.6338</v>
+        <v>1354.686</v>
       </c>
       <c r="M6" t="n">
-        <v>77.72693</v>
+        <v>66.04146</v>
       </c>
       <c r="N6" t="n">
-        <v>3640733</v>
+        <v>3905571</v>
       </c>
       <c r="O6" t="n">
-        <v>10588.75</v>
+        <v>8566.797</v>
       </c>
       <c r="P6" t="n">
-        <v>1004.607</v>
+        <v>274.5239</v>
       </c>
       <c r="Q6" t="n">
-        <v>2598.249</v>
+        <v>2170.566</v>
       </c>
       <c r="R6" t="n">
-        <v>76.67639</v>
+        <v>137.1645</v>
       </c>
       <c r="S6" t="n">
-        <v>90.43989999999999</v>
+        <v>77.10662000000001</v>
       </c>
       <c r="T6" t="n">
-        <v>64933.62</v>
+        <v>28401.01</v>
       </c>
       <c r="U6" t="n">
-        <v>541.2913</v>
+        <v>2586.657</v>
       </c>
       <c r="V6" t="n">
-        <v>133.3401</v>
+        <v>107.396</v>
       </c>
       <c r="W6" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X6" t="n">
-        <v>1438.781</v>
+        <v>180.3007</v>
       </c>
       <c r="Y6" t="n">
-        <v>334.5619</v>
+        <v>339.819</v>
       </c>
       <c r="Z6" t="n">
-        <v>370.5425</v>
+        <v>383.6598</v>
       </c>
       <c r="AA6" t="n">
-        <v>457.2187</v>
+        <v>437.8539</v>
       </c>
       <c r="AB6" t="n">
-        <v>949.353</v>
+        <v>697.7505</v>
       </c>
       <c r="AC6" t="n">
-        <v>399.1537</v>
+        <v>400.4562</v>
       </c>
       <c r="AD6" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE6" t="n">
-        <v>307.1879</v>
+        <v>369.2915</v>
       </c>
       <c r="AF6" t="n">
-        <v>850767.7</v>
+        <v>876990.5</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>70823040</v>
+        <v>27668500</v>
       </c>
       <c r="D7" t="n">
-        <v>5276534</v>
+        <v>2325621</v>
       </c>
       <c r="E7" t="n">
-        <v>2916.64</v>
+        <v>18559.01</v>
       </c>
       <c r="F7" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G7" t="n">
-        <v>34.17702</v>
+        <v>48.22939</v>
       </c>
       <c r="H7" t="n">
-        <v>27.26317</v>
+        <v>21.9057</v>
       </c>
       <c r="I7" t="n">
-        <v>74.63590000000001</v>
+        <v>96.65864999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>45.38999</v>
+        <v>41.79208</v>
       </c>
       <c r="K7" t="n">
-        <v>405.2997</v>
+        <v>157.3232</v>
       </c>
       <c r="L7" t="n">
-        <v>997.6338</v>
+        <v>1185.157</v>
       </c>
       <c r="M7" t="n">
-        <v>77.72693</v>
+        <v>66.04146</v>
       </c>
       <c r="N7" t="n">
-        <v>3640733</v>
+        <v>3823828</v>
       </c>
       <c r="O7" t="n">
-        <v>7191.416</v>
+        <v>8566.797</v>
       </c>
       <c r="P7" t="n">
-        <v>819.2155</v>
+        <v>274.5239</v>
       </c>
       <c r="Q7" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R7" t="n">
-        <v>76.67639</v>
+        <v>137.1645</v>
       </c>
       <c r="S7" t="n">
-        <v>82.65521</v>
+        <v>77.10662000000001</v>
       </c>
       <c r="T7" t="n">
-        <v>20540.78</v>
+        <v>28401.01</v>
       </c>
       <c r="U7" t="n">
-        <v>541.2913</v>
+        <v>1078.603</v>
       </c>
       <c r="V7" t="n">
-        <v>127.3378</v>
+        <v>107.396</v>
       </c>
       <c r="W7" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X7" t="n">
-        <v>118.8049</v>
+        <v>180.3007</v>
       </c>
       <c r="Y7" t="n">
-        <v>334.5619</v>
+        <v>336.3015</v>
       </c>
       <c r="Z7" t="n">
-        <v>370.5425</v>
+        <v>198.3025</v>
       </c>
       <c r="AA7" t="n">
-        <v>452.2695</v>
+        <v>437.8539</v>
       </c>
       <c r="AB7" t="n">
-        <v>949.353</v>
+        <v>630.905</v>
       </c>
       <c r="AC7" t="n">
-        <v>399.1537</v>
+        <v>399.9794</v>
       </c>
       <c r="AD7" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE7" t="n">
-        <v>300.3805</v>
+        <v>277.5095</v>
       </c>
       <c r="AF7" t="n">
-        <v>808515.8</v>
+        <v>760823.6</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>70823040</v>
+        <v>27668500</v>
       </c>
       <c r="D8" t="n">
-        <v>1042477</v>
+        <v>1929561</v>
       </c>
       <c r="E8" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F8" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G8" t="n">
-        <v>34.17702</v>
+        <v>43.40393</v>
       </c>
       <c r="H8" t="n">
-        <v>26.12377</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J8" t="n">
-        <v>45.38999</v>
+        <v>41.79208</v>
       </c>
       <c r="K8" t="n">
-        <v>405.2997</v>
+        <v>157.3232</v>
       </c>
       <c r="L8" t="n">
-        <v>997.6338</v>
+        <v>1185.157</v>
       </c>
       <c r="M8" t="n">
-        <v>23.44354</v>
+        <v>66.04146</v>
       </c>
       <c r="N8" t="n">
-        <v>3377673</v>
+        <v>3823828</v>
       </c>
       <c r="O8" t="n">
-        <v>3260.107</v>
+        <v>5491.206</v>
       </c>
       <c r="P8" t="n">
-        <v>290.8183</v>
+        <v>274.5239</v>
       </c>
       <c r="Q8" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R8" t="n">
-        <v>76.67639</v>
+        <v>137.1645</v>
       </c>
       <c r="S8" t="n">
-        <v>77.37721000000001</v>
+        <v>61.51114</v>
       </c>
       <c r="T8" t="n">
-        <v>20540.78</v>
+        <v>28401.01</v>
       </c>
       <c r="U8" t="n">
-        <v>541.2913</v>
+        <v>961.4151000000001</v>
       </c>
       <c r="V8" t="n">
-        <v>127.3378</v>
+        <v>107.396</v>
       </c>
       <c r="W8" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X8" t="n">
-        <v>118.8049</v>
+        <v>180.3007</v>
       </c>
       <c r="Y8" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z8" t="n">
-        <v>368.4272</v>
+        <v>198.3025</v>
       </c>
       <c r="AA8" t="n">
-        <v>449.7888</v>
+        <v>437.8539</v>
       </c>
       <c r="AB8" t="n">
-        <v>573.0429</v>
+        <v>630.905</v>
       </c>
       <c r="AC8" t="n">
-        <v>399.1537</v>
+        <v>399.9794</v>
       </c>
       <c r="AD8" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE8" t="n">
-        <v>300.3805</v>
+        <v>277.5095</v>
       </c>
       <c r="AF8" t="n">
-        <v>803157.7</v>
+        <v>702338.3</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>53990370</v>
+        <v>17370480</v>
       </c>
       <c r="D9" t="n">
-        <v>1042477</v>
+        <v>1929561</v>
       </c>
       <c r="E9" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F9" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G9" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H9" t="n">
-        <v>18.73368</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J9" t="n">
-        <v>45.38999</v>
+        <v>41.79208</v>
       </c>
       <c r="K9" t="n">
-        <v>352.9796</v>
+        <v>157.3232</v>
       </c>
       <c r="L9" t="n">
-        <v>997.3243</v>
+        <v>1052.64</v>
       </c>
       <c r="M9" t="n">
-        <v>23.44354</v>
+        <v>66.04146</v>
       </c>
       <c r="N9" t="n">
-        <v>3377673</v>
+        <v>3823828</v>
       </c>
       <c r="O9" t="n">
-        <v>3260.107</v>
+        <v>5491.206</v>
       </c>
       <c r="P9" t="n">
-        <v>290.8183</v>
+        <v>274.5239</v>
       </c>
       <c r="Q9" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R9" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S9" t="n">
-        <v>77.37721000000001</v>
+        <v>61.51114</v>
       </c>
       <c r="T9" t="n">
-        <v>20540.78</v>
+        <v>28401.01</v>
       </c>
       <c r="U9" t="n">
-        <v>291.0584</v>
+        <v>961.4151000000001</v>
       </c>
       <c r="V9" t="n">
-        <v>127.3378</v>
+        <v>107.396</v>
       </c>
       <c r="W9" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X9" t="n">
-        <v>118.8049</v>
+        <v>142.3543</v>
       </c>
       <c r="Y9" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z9" t="n">
-        <v>368.4272</v>
+        <v>198.3025</v>
       </c>
       <c r="AA9" t="n">
-        <v>449.7888</v>
+        <v>414.9175</v>
       </c>
       <c r="AB9" t="n">
-        <v>531.1274</v>
+        <v>630.905</v>
       </c>
       <c r="AC9" t="n">
-        <v>399.1537</v>
+        <v>399.9794</v>
       </c>
       <c r="AD9" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE9" t="n">
-        <v>300.3805</v>
+        <v>277.5095</v>
       </c>
       <c r="AF9" t="n">
-        <v>793688.8</v>
+        <v>702338.3</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>53990370</v>
+        <v>17370480</v>
       </c>
       <c r="D10" t="n">
-        <v>1042477</v>
+        <v>1929561</v>
       </c>
       <c r="E10" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F10" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G10" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H10" t="n">
-        <v>18.73368</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I10" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J10" t="n">
-        <v>45.38999</v>
+        <v>41.79208</v>
       </c>
       <c r="K10" t="n">
-        <v>352.9796</v>
+        <v>127.0489</v>
       </c>
       <c r="L10" t="n">
-        <v>997.3243</v>
+        <v>1050.769</v>
       </c>
       <c r="M10" t="n">
-        <v>23.44354</v>
+        <v>66.04146</v>
       </c>
       <c r="N10" t="n">
-        <v>3377673</v>
+        <v>2111865</v>
       </c>
       <c r="O10" t="n">
-        <v>2136.811</v>
+        <v>5491.206</v>
       </c>
       <c r="P10" t="n">
-        <v>151.15</v>
+        <v>274.5239</v>
       </c>
       <c r="Q10" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R10" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S10" t="n">
-        <v>77.37721000000001</v>
+        <v>61.51114</v>
       </c>
       <c r="T10" t="n">
-        <v>20540.78</v>
+        <v>28401.01</v>
       </c>
       <c r="U10" t="n">
-        <v>291.0584</v>
+        <v>961.4151000000001</v>
       </c>
       <c r="V10" t="n">
-        <v>127.3378</v>
+        <v>105.7336</v>
       </c>
       <c r="W10" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X10" t="n">
-        <v>118.8049</v>
+        <v>142.3543</v>
       </c>
       <c r="Y10" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z10" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA10" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB10" t="n">
-        <v>481.9967</v>
+        <v>630.905</v>
       </c>
       <c r="AC10" t="n">
-        <v>399.1537</v>
+        <v>399.9794</v>
       </c>
       <c r="AD10" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE10" t="n">
-        <v>300.3805</v>
+        <v>277.5095</v>
       </c>
       <c r="AF10" t="n">
-        <v>793688.8</v>
+        <v>680184.4</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>53990370</v>
+        <v>17370480</v>
       </c>
       <c r="D11" t="n">
-        <v>93985</v>
+        <v>1929561</v>
       </c>
       <c r="E11" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F11" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G11" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H11" t="n">
-        <v>18.73368</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I11" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J11" t="n">
-        <v>45.38999</v>
+        <v>38.97002</v>
       </c>
       <c r="K11" t="n">
-        <v>333.1313</v>
+        <v>127.0489</v>
       </c>
       <c r="L11" t="n">
-        <v>997.3243</v>
+        <v>1050.769</v>
       </c>
       <c r="M11" t="n">
-        <v>23.44354</v>
+        <v>66.04146</v>
       </c>
       <c r="N11" t="n">
-        <v>3377673</v>
+        <v>1113412</v>
       </c>
       <c r="O11" t="n">
-        <v>1868.794</v>
+        <v>4282.262</v>
       </c>
       <c r="P11" t="n">
-        <v>151.15</v>
+        <v>88.83244000000001</v>
       </c>
       <c r="Q11" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R11" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S11" t="n">
-        <v>74.25953</v>
+        <v>61.51114</v>
       </c>
       <c r="T11" t="n">
-        <v>20540.78</v>
+        <v>28401.01</v>
       </c>
       <c r="U11" t="n">
-        <v>291.0584</v>
+        <v>961.4151000000001</v>
       </c>
       <c r="V11" t="n">
-        <v>126.9379</v>
+        <v>95.22617</v>
       </c>
       <c r="W11" t="n">
-        <v>121.6149</v>
+        <v>109.833</v>
       </c>
       <c r="X11" t="n">
-        <v>118.8049</v>
+        <v>142.3543</v>
       </c>
       <c r="Y11" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z11" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA11" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB11" t="n">
-        <v>481.9967</v>
+        <v>567.9717000000001</v>
       </c>
       <c r="AC11" t="n">
-        <v>399.1537</v>
+        <v>393.7578</v>
       </c>
       <c r="AD11" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE11" t="n">
-        <v>299.7434</v>
+        <v>277.5095</v>
       </c>
       <c r="AF11" t="n">
-        <v>793688.8</v>
+        <v>680184.4</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>32660020</v>
+        <v>17370480</v>
       </c>
       <c r="D12" t="n">
-        <v>93985</v>
+        <v>1929561</v>
       </c>
       <c r="E12" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F12" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G12" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H12" t="n">
-        <v>18.73368</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I12" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J12" t="n">
-        <v>34.70593</v>
+        <v>38.97002</v>
       </c>
       <c r="K12" t="n">
-        <v>211.6953</v>
+        <v>127.0489</v>
       </c>
       <c r="L12" t="n">
-        <v>997.3243</v>
+        <v>1050.769</v>
       </c>
       <c r="M12" t="n">
-        <v>23.44354</v>
+        <v>60.36494</v>
       </c>
       <c r="N12" t="n">
-        <v>3377673</v>
+        <v>1113412</v>
       </c>
       <c r="O12" t="n">
-        <v>1868.794</v>
+        <v>4282.262</v>
       </c>
       <c r="P12" t="n">
-        <v>151.15</v>
+        <v>88.83244000000001</v>
       </c>
       <c r="Q12" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R12" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S12" t="n">
-        <v>60.10981</v>
+        <v>61.51114</v>
       </c>
       <c r="T12" t="n">
-        <v>20540.78</v>
+        <v>18826.29</v>
       </c>
       <c r="U12" t="n">
-        <v>291.0584</v>
+        <v>737.3378</v>
       </c>
       <c r="V12" t="n">
-        <v>126.9379</v>
+        <v>95.22617</v>
       </c>
       <c r="W12" t="n">
-        <v>109.6236</v>
+        <v>107.3324</v>
       </c>
       <c r="X12" t="n">
-        <v>118.8049</v>
+        <v>142.3543</v>
       </c>
       <c r="Y12" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z12" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA12" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB12" t="n">
-        <v>481.9967</v>
+        <v>567.9717000000001</v>
       </c>
       <c r="AC12" t="n">
-        <v>398.2069</v>
+        <v>393.7578</v>
       </c>
       <c r="AD12" t="n">
-        <v>451.3176</v>
+        <v>611.7071</v>
       </c>
       <c r="AE12" t="n">
-        <v>299.7434</v>
+        <v>277.5095</v>
       </c>
       <c r="AF12" t="n">
-        <v>793688.8</v>
+        <v>680184.4</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>32660020</v>
+        <v>17370480</v>
       </c>
       <c r="D13" t="n">
-        <v>93985</v>
+        <v>1929561</v>
       </c>
       <c r="E13" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F13" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G13" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H13" t="n">
-        <v>16.34718</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I13" t="n">
-        <v>74.63590000000001</v>
+        <v>82.46593</v>
       </c>
       <c r="J13" t="n">
-        <v>34.70593</v>
+        <v>38.97002</v>
       </c>
       <c r="K13" t="n">
-        <v>211.6953</v>
+        <v>127.0489</v>
       </c>
       <c r="L13" t="n">
-        <v>997.3243</v>
+        <v>1050.769</v>
       </c>
       <c r="M13" t="n">
-        <v>23.44354</v>
+        <v>60.36494</v>
       </c>
       <c r="N13" t="n">
-        <v>3171403</v>
+        <v>1113412</v>
       </c>
       <c r="O13" t="n">
-        <v>1868.794</v>
+        <v>4282.262</v>
       </c>
       <c r="P13" t="n">
-        <v>151.15</v>
+        <v>88.83244000000001</v>
       </c>
       <c r="Q13" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R13" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S13" t="n">
-        <v>60.10981</v>
+        <v>61.51114</v>
       </c>
       <c r="T13" t="n">
-        <v>20540.78</v>
+        <v>18826.29</v>
       </c>
       <c r="U13" t="n">
-        <v>291.0584</v>
+        <v>639.1803</v>
       </c>
       <c r="V13" t="n">
-        <v>126.9379</v>
+        <v>95.22617</v>
       </c>
       <c r="W13" t="n">
-        <v>109.6236</v>
+        <v>107.3324</v>
       </c>
       <c r="X13" t="n">
-        <v>118.8049</v>
+        <v>142.3543</v>
       </c>
       <c r="Y13" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z13" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA13" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB13" t="n">
-        <v>481.9967</v>
+        <v>567.9717000000001</v>
       </c>
       <c r="AC13" t="n">
-        <v>398.2069</v>
+        <v>393.7578</v>
       </c>
       <c r="AD13" t="n">
-        <v>451.3176</v>
+        <v>515.703</v>
       </c>
       <c r="AE13" t="n">
-        <v>299.7434</v>
+        <v>277.5095</v>
       </c>
       <c r="AF13" t="n">
-        <v>793688.8</v>
+        <v>622060.9</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>32660020</v>
+        <v>17370480</v>
       </c>
       <c r="D14" t="n">
-        <v>93985</v>
+        <v>1929561</v>
       </c>
       <c r="E14" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F14" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G14" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H14" t="n">
-        <v>16.34718</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I14" t="n">
-        <v>67.40559</v>
+        <v>82.46593</v>
       </c>
       <c r="J14" t="n">
-        <v>34.70593</v>
+        <v>38.97002</v>
       </c>
       <c r="K14" t="n">
-        <v>211.6953</v>
+        <v>127.0489</v>
       </c>
       <c r="L14" t="n">
-        <v>997.3243</v>
+        <v>1050.769</v>
       </c>
       <c r="M14" t="n">
-        <v>23.44354</v>
+        <v>60.36494</v>
       </c>
       <c r="N14" t="n">
-        <v>3171403</v>
+        <v>1113412</v>
       </c>
       <c r="O14" t="n">
-        <v>1868.794</v>
+        <v>4282.262</v>
       </c>
       <c r="P14" t="n">
-        <v>151.15</v>
+        <v>88.83244000000001</v>
       </c>
       <c r="Q14" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R14" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S14" t="n">
-        <v>60.10981</v>
+        <v>61.51114</v>
       </c>
       <c r="T14" t="n">
-        <v>5720.186</v>
+        <v>18826.29</v>
       </c>
       <c r="U14" t="n">
-        <v>291.0584</v>
+        <v>639.1803</v>
       </c>
       <c r="V14" t="n">
-        <v>117.4828</v>
+        <v>91.61051999999999</v>
       </c>
       <c r="W14" t="n">
-        <v>109.6236</v>
+        <v>107.3324</v>
       </c>
       <c r="X14" t="n">
-        <v>118.8049</v>
+        <v>130.1473</v>
       </c>
       <c r="Y14" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z14" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA14" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB14" t="n">
-        <v>481.9967</v>
+        <v>567.9717000000001</v>
       </c>
       <c r="AC14" t="n">
-        <v>398.2069</v>
+        <v>393.7578</v>
       </c>
       <c r="AD14" t="n">
-        <v>439.7913</v>
+        <v>500.6479</v>
       </c>
       <c r="AE14" t="n">
-        <v>299.7434</v>
+        <v>277.5095</v>
       </c>
       <c r="AF14" t="n">
-        <v>793688.8</v>
+        <v>622060.9</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>32660020</v>
+        <v>17370480</v>
       </c>
       <c r="D15" t="n">
-        <v>93985</v>
+        <v>1929561</v>
       </c>
       <c r="E15" t="n">
-        <v>2916.64</v>
+        <v>10041.54</v>
       </c>
       <c r="F15" t="n">
-        <v>19.6207</v>
+        <v>16.92496</v>
       </c>
       <c r="G15" t="n">
-        <v>34.17702</v>
+        <v>25.6849</v>
       </c>
       <c r="H15" t="n">
-        <v>15.85893</v>
+        <v>9.444687999999999</v>
       </c>
       <c r="I15" t="n">
-        <v>67.40559</v>
+        <v>82.46593</v>
       </c>
       <c r="J15" t="n">
-        <v>34.70593</v>
+        <v>38.97002</v>
       </c>
       <c r="K15" t="n">
-        <v>211.6953</v>
+        <v>127.0489</v>
       </c>
       <c r="L15" t="n">
-        <v>811.7886999999999</v>
+        <v>970.4228000000001</v>
       </c>
       <c r="M15" t="n">
-        <v>23.44354</v>
+        <v>60.36494</v>
       </c>
       <c r="N15" t="n">
-        <v>876271.7</v>
+        <v>236724.5</v>
       </c>
       <c r="O15" t="n">
-        <v>1868.794</v>
+        <v>4282.262</v>
       </c>
       <c r="P15" t="n">
-        <v>151.15</v>
+        <v>88.83244000000001</v>
       </c>
       <c r="Q15" t="n">
-        <v>667.6783</v>
+        <v>2142.696</v>
       </c>
       <c r="R15" t="n">
-        <v>55.93324</v>
+        <v>35.19613</v>
       </c>
       <c r="S15" t="n">
-        <v>60.10981</v>
+        <v>61.51114</v>
       </c>
       <c r="T15" t="n">
-        <v>5720.186</v>
+        <v>18826.29</v>
       </c>
       <c r="U15" t="n">
-        <v>291.0584</v>
+        <v>639.1803</v>
       </c>
       <c r="V15" t="n">
-        <v>92.86722</v>
+        <v>91.61051999999999</v>
       </c>
       <c r="W15" t="n">
-        <v>109.6236</v>
+        <v>107.3324</v>
       </c>
       <c r="X15" t="n">
-        <v>85.71588</v>
+        <v>130.1473</v>
       </c>
       <c r="Y15" t="n">
-        <v>325.0987</v>
+        <v>330.3065</v>
       </c>
       <c r="Z15" t="n">
-        <v>178.592</v>
+        <v>198.3025</v>
       </c>
       <c r="AA15" t="n">
-        <v>425.7462</v>
+        <v>414.9175</v>
       </c>
       <c r="AB15" t="n">
-        <v>481.9967</v>
+        <v>567.9717000000001</v>
       </c>
       <c r="AC15" t="n">
-        <v>398.2069</v>
+        <v>393.7578</v>
       </c>
       <c r="AD15" t="n">
-        <v>436.2223</v>
+        <v>407.2273</v>
       </c>
       <c r="AE15" t="n">
-        <v>299.7434</v>
+        <v>277.5095</v>
       </c>
       <c r="AF15" t="n">
-        <v>746620.8</v>
+        <v>247804.9</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>